<commit_message>
Add tie breaking rule to EMSC stats calculation
</commit_message>
<xml_diff>
--- a/EMSC Stats Test 2.xlsx
+++ b/EMSC Stats Test 2.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -418,6 +418,8 @@
     <col min="14" max="14" customWidth="1" width="13"/>
     <col min="15" max="15" customWidth="1" width="14"/>
     <col min="16" max="16" customWidth="1" width="12"/>
+    <col min="17" max="17" customWidth="1" width="18"/>
+    <col min="18" max="18" customWidth="1" width="17"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -469,6 +471,12 @@
       <c r="P1" t="str">
         <v>Is Finalist</v>
       </c>
+      <c r="Q1" t="str">
+        <v>Final Points From</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Semi Points From</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -1628,7 +1636,7 @@
         <v>EMSC2304</v>
       </c>
       <c r="C25" t="str">
-        <v>Marocco</v>
+        <v>Morocco</v>
       </c>
       <c r="D25" t="str">
         <v>ABIR</v>
@@ -1728,16 +1736,16 @@
         <v>EMSC2304</v>
       </c>
       <c r="C27" t="str">
-        <v>Estonia</v>
+        <v>Poland</v>
       </c>
       <c r="D27" t="str">
-        <v>Liis Lemsalu</v>
+        <v>Viki Gabor</v>
       </c>
       <c r="E27" t="str">
-        <v>Kehakeel</v>
+        <v>Barbie</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" t="str">
         <v/>
@@ -1749,10 +1757,10 @@
         <v>13</v>
       </c>
       <c r="J27">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="K27" t="str">
-        <v>Mathias</v>
+        <v>Luke</v>
       </c>
       <c r="L27" t="str">
         <v/>
@@ -1761,7 +1769,7 @@
         <v/>
       </c>
       <c r="N27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O27" t="str">
         <v/>
@@ -1778,16 +1786,16 @@
         <v>EMSC2304</v>
       </c>
       <c r="C28" t="str">
-        <v>Romania</v>
+        <v>Montenegro</v>
       </c>
       <c r="D28" t="str">
-        <v>WRS</v>
+        <v>Emel</v>
       </c>
       <c r="E28" t="str">
-        <v>Dale</v>
+        <v>Gdje je</v>
       </c>
       <c r="F28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G28" t="str">
         <v/>
@@ -1799,10 +1807,10 @@
         <v>14</v>
       </c>
       <c r="J28">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="K28" t="str">
-        <v>Edu Padr\u00f3s Creus</v>
+        <v>Rodrigo  Erazo</v>
       </c>
       <c r="L28" t="str">
         <v/>
@@ -1811,7 +1819,7 @@
         <v/>
       </c>
       <c r="N28">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O28" t="str">
         <v/>
@@ -1828,16 +1836,16 @@
         <v>EMSC2304</v>
       </c>
       <c r="C29" t="str">
-        <v>Azerbaijan</v>
+        <v>Georgia</v>
       </c>
       <c r="D29" t="str">
-        <v>R\u00f6ya &amp; Nicat R\u0259himov</v>
+        <v>Katie Melua</v>
       </c>
       <c r="E29" t="str">
-        <v>D\u0259li kimi</v>
+        <v>A love like that</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G29" t="str">
         <v/>
@@ -1846,13 +1854,13 @@
         <v/>
       </c>
       <c r="I29">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J29">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K29" t="str">
-        <v>Nijat</v>
+        <v>Richard Cox</v>
       </c>
       <c r="L29" t="str">
         <v/>
@@ -1861,7 +1869,7 @@
         <v/>
       </c>
       <c r="N29">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O29" t="str">
         <v/>
@@ -1878,16 +1886,16 @@
         <v>EMSC2304</v>
       </c>
       <c r="C30" t="str">
-        <v>Greece</v>
+        <v>Ukraine</v>
       </c>
       <c r="D30" t="str">
-        <v>ZAF</v>
+        <v>Ruma</v>
       </c>
       <c r="E30" t="str">
-        <v>Pes</v>
+        <v>\u0414\u043e\u0442\u0438\u043a</v>
       </c>
       <c r="F30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G30" t="str">
         <v/>
@@ -1896,13 +1904,13 @@
         <v/>
       </c>
       <c r="I30">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J30">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="K30" t="str">
-        <v>Christoforos Andrianos</v>
+        <v>Lu\u00eds Coelho</v>
       </c>
       <c r="L30" t="str">
         <v/>
@@ -1911,7 +1919,7 @@
         <v/>
       </c>
       <c r="N30">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="O30" t="str">
         <v/>
@@ -1928,13 +1936,13 @@
         <v>EMSC2304</v>
       </c>
       <c r="C31" t="str">
-        <v>Moldova, Republic of</v>
+        <v>Estonia</v>
       </c>
       <c r="D31" t="str">
-        <v>Vanotek &amp; Eneli</v>
+        <v>Liis Lemsalu</v>
       </c>
       <c r="E31" t="str">
-        <v>Back to me</v>
+        <v>Kehakeel</v>
       </c>
       <c r="F31">
         <v>2</v>
@@ -1946,13 +1954,13 @@
         <v/>
       </c>
       <c r="I31">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J31">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K31" t="str">
-        <v>FabioMassimo</v>
+        <v>Mathias</v>
       </c>
       <c r="L31" t="str">
         <v/>
@@ -1961,7 +1969,7 @@
         <v/>
       </c>
       <c r="N31">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="O31" t="str">
         <v/>
@@ -1978,16 +1986,16 @@
         <v>EMSC2304</v>
       </c>
       <c r="C32" t="str">
-        <v>Poland</v>
+        <v>Romania</v>
       </c>
       <c r="D32" t="str">
-        <v>Viki Gabor</v>
+        <v>WRS</v>
       </c>
       <c r="E32" t="str">
-        <v>Barbie</v>
+        <v>Dale</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G32" t="str">
         <v/>
@@ -1996,13 +2004,13 @@
         <v/>
       </c>
       <c r="I32">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J32">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="K32" t="str">
-        <v>Luke</v>
+        <v>Edu Padr\u00f3s Creus</v>
       </c>
       <c r="L32" t="str">
         <v/>
@@ -2028,16 +2036,16 @@
         <v>EMSC2304</v>
       </c>
       <c r="C33" t="str">
-        <v>Montenegro</v>
+        <v>Moldova</v>
       </c>
       <c r="D33" t="str">
-        <v>Emel</v>
+        <v>Vanotek &amp; Eneli</v>
       </c>
       <c r="E33" t="str">
-        <v>Gdje je</v>
+        <v>Back to me</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G33" t="str">
         <v/>
@@ -2046,13 +2054,13 @@
         <v/>
       </c>
       <c r="I33">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J33">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="K33" t="str">
-        <v>Rodrigo  Erazo</v>
+        <v>FabioMassimo</v>
       </c>
       <c r="L33" t="str">
         <v/>
@@ -2061,7 +2069,7 @@
         <v/>
       </c>
       <c r="N33">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="O33" t="str">
         <v/>
@@ -2078,16 +2086,16 @@
         <v>EMSC2304</v>
       </c>
       <c r="C34" t="str">
-        <v>Georgia</v>
+        <v>Azerbaijan</v>
       </c>
       <c r="D34" t="str">
-        <v>Katie Melua</v>
+        <v>R\u00f6ya &amp; Nicat R\u0259himov</v>
       </c>
       <c r="E34" t="str">
-        <v>A love like that</v>
+        <v>D\u0259li kimi</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G34" t="str">
         <v/>
@@ -2096,13 +2104,13 @@
         <v/>
       </c>
       <c r="I34">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J34">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K34" t="str">
-        <v>Richard Cox</v>
+        <v>Nijat</v>
       </c>
       <c r="L34" t="str">
         <v/>
@@ -2111,7 +2119,7 @@
         <v/>
       </c>
       <c r="N34">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O34" t="str">
         <v/>
@@ -2128,16 +2136,16 @@
         <v>EMSC2304</v>
       </c>
       <c r="C35" t="str">
-        <v>Ukraine</v>
+        <v>Greece</v>
       </c>
       <c r="D35" t="str">
-        <v>Ruma</v>
+        <v>ZAF</v>
       </c>
       <c r="E35" t="str">
-        <v>\u0414\u043e\u0442\u0438\u043a</v>
+        <v>Pes</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G35" t="str">
         <v/>
@@ -2146,13 +2154,13 @@
         <v/>
       </c>
       <c r="I35">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J35">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="K35" t="str">
-        <v>Lu\u00eds Coelho</v>
+        <v>Christoforos Andrianos</v>
       </c>
       <c r="L35" t="str">
         <v/>
@@ -2161,7 +2169,7 @@
         <v/>
       </c>
       <c r="N35">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O35" t="str">
         <v/>
@@ -2172,7 +2180,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:P35"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:R35"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>